<commit_message>
Actualizacion historias de usuario en cronogrma
</commit_message>
<xml_diff>
--- a/Documentos/SF/Cronograma/Cronograma de Proyecto.xlsx
+++ b/Documentos/SF/Cronograma/Cronograma de Proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\wong\FiveSolutions\Documentos\SF\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE832624-2826-4C09-955B-0BA6B8782C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF46AE-807B-46CF-9684-A7B31F916288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="132">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -189,9 +189,6 @@
     <t>ST-PP.DOCX</t>
   </si>
   <si>
-    <t>Correa/Diseñador, Yantas/FE. Flores/FE</t>
-  </si>
-  <si>
     <t>Analista de software</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Tello/DBA, Benavente/BE, Yantas/FE. Flores/FE</t>
-  </si>
-  <si>
     <t>Integración Frontend-Backend</t>
   </si>
   <si>
@@ -282,9 +276,6 @@
     <t>ST-SP.DOCX</t>
   </si>
   <si>
-    <t>Correa/Diseñador, Yantas/FE</t>
-  </si>
-  <si>
     <t>HU-Registrar, actualizar y/o eliminar producto</t>
   </si>
   <si>
@@ -424,6 +415,12 @@
   </si>
   <si>
     <t>ST-MB.DOCX</t>
+  </si>
+  <si>
+    <t>Correa/Diseñador</t>
+  </si>
+  <si>
+    <t>Tello/DBA, Benavente/BE, Flores/FE</t>
   </si>
 </sst>
 </file>
@@ -433,7 +430,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,6 +482,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -584,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -637,6 +647,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -645,11 +660,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -888,15 +902,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="14.4">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="2:16" ht="14.4">
       <c r="B2" s="1" t="s">
@@ -968,10 +982,10 @@
       <c r="H8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="39"/>
+      <c r="K8" s="42"/>
       <c r="L8" s="8"/>
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
@@ -1178,8 +1192,8 @@
       <c r="D15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>54</v>
+      <c r="E15" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="F15" s="21">
         <v>44359</v>
@@ -1189,10 +1203,10 @@
       </c>
       <c r="H15" s="17"/>
       <c r="J15" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="16" t="s">
         <v>55</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>56</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="9"/>
@@ -1202,16 +1216,16 @@
     </row>
     <row r="16" spans="2:16" ht="14.4">
       <c r="B16" s="19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C16" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="E16" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>59</v>
       </c>
       <c r="F16" s="21">
         <v>44363</v>
@@ -1221,10 +1235,10 @@
       </c>
       <c r="H16" s="17"/>
       <c r="J16" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="22" t="s">
         <v>60</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>61</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="9"/>
@@ -1234,16 +1248,16 @@
     </row>
     <row r="17" spans="2:16" s="35" customFormat="1" ht="14.4">
       <c r="B17" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="D17" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>122</v>
-      </c>
       <c r="E17" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" s="21">
         <v>44363</v>
@@ -1252,8 +1266,8 @@
         <v>44368</v>
       </c>
       <c r="H17" s="17"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="41"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="37"/>
       <c r="L17" s="8"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
@@ -1262,16 +1276,16 @@
     </row>
     <row r="18" spans="2:16" s="35" customFormat="1" ht="14.4">
       <c r="B18" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="D18" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>123</v>
-      </c>
       <c r="E18" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="21">
         <v>44363</v>
@@ -1280,8 +1294,8 @@
         <v>44368</v>
       </c>
       <c r="H18" s="17"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="41"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="37"/>
       <c r="L18" s="8"/>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
@@ -1290,16 +1304,16 @@
     </row>
     <row r="19" spans="2:16" s="35" customFormat="1" ht="14.4">
       <c r="B19" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="D19" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>124</v>
-      </c>
       <c r="E19" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F19" s="21">
         <v>44363</v>
@@ -1308,8 +1322,8 @@
         <v>44368</v>
       </c>
       <c r="H19" s="17"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="41"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="37"/>
       <c r="L19" s="8"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
@@ -1318,16 +1332,16 @@
     </row>
     <row r="20" spans="2:16" ht="14.4">
       <c r="B20" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="D20" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>64</v>
-      </c>
       <c r="E20" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" s="21">
         <v>44363</v>
@@ -1346,16 +1360,16 @@
     </row>
     <row r="21" spans="2:16" ht="14.4">
       <c r="B21" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>131</v>
       </c>
       <c r="F21" s="21">
         <v>44367</v>
@@ -1374,16 +1388,16 @@
     </row>
     <row r="22" spans="2:16" ht="14.4">
       <c r="B22" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F22" s="21">
         <v>44368</v>
@@ -1402,16 +1416,16 @@
     </row>
     <row r="23" spans="2:16" ht="14.4">
       <c r="B23" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F23" s="21">
         <v>44370</v>
@@ -1430,16 +1444,16 @@
     </row>
     <row r="24" spans="2:16" ht="14.4">
       <c r="B24" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F24" s="21">
         <v>44373</v>
@@ -1451,16 +1465,16 @@
     </row>
     <row r="25" spans="2:16" ht="14.4">
       <c r="B25" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F25" s="21">
         <v>44375</v>
@@ -1472,13 +1486,13 @@
     </row>
     <row r="26" spans="2:16" ht="14.4">
       <c r="B26" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>25</v>
@@ -1493,13 +1507,13 @@
     </row>
     <row r="27" spans="2:16" ht="14.4">
       <c r="B27" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>25</v>
@@ -1514,7 +1528,7 @@
     </row>
     <row r="28" spans="2:16" ht="14.4">
       <c r="B28" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="24"/>
@@ -1525,7 +1539,7 @@
     </row>
     <row r="29" spans="2:16" ht="14.4">
       <c r="B29" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -1536,13 +1550,13 @@
     </row>
     <row r="30" spans="2:16" ht="15.75" customHeight="1">
       <c r="B30" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>81</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>25</v>
@@ -1557,16 +1571,16 @@
     </row>
     <row r="31" spans="2:16" ht="15.75" customHeight="1">
       <c r="B31" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>85</v>
+      <c r="E31" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="F31" s="4">
         <v>44380</v>
@@ -1577,17 +1591,17 @@
       <c r="H31" s="27"/>
     </row>
     <row r="32" spans="2:16" s="35" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B32" s="42" t="s">
-        <v>125</v>
+      <c r="B32" s="38" t="s">
+        <v>122</v>
       </c>
       <c r="C32" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D32" s="18" t="s">
-        <v>130</v>
-      </c>
       <c r="E32" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F32" s="4">
         <v>44380</v>
@@ -1598,17 +1612,17 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B33" s="42" t="s">
-        <v>86</v>
+      <c r="B33" s="38" t="s">
+        <v>83</v>
       </c>
       <c r="C33" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="18" t="s">
-        <v>131</v>
-      </c>
       <c r="E33" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F33" s="4">
         <v>44380</v>
@@ -1619,17 +1633,17 @@
       <c r="H33" s="27"/>
     </row>
     <row r="34" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="D34" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D34" s="18" t="s">
-        <v>132</v>
-      </c>
       <c r="E34" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F34" s="4">
         <v>44380</v>
@@ -1641,16 +1655,16 @@
     </row>
     <row r="35" spans="2:8" ht="15.75" customHeight="1">
       <c r="B35" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F35" s="21">
         <v>44397</v>
@@ -1662,16 +1676,16 @@
     </row>
     <row r="36" spans="2:8" ht="15.75" customHeight="1">
       <c r="B36" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>88</v>
+        <v>65</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>85</v>
       </c>
       <c r="F36" s="21">
         <v>44398</v>
@@ -1683,16 +1697,16 @@
     </row>
     <row r="37" spans="2:8" ht="15.75" customHeight="1">
       <c r="B37" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F37" s="21">
         <v>44400</v>
@@ -1704,16 +1718,16 @@
     </row>
     <row r="38" spans="2:8" ht="15.75" customHeight="1">
       <c r="B38" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F38" s="21">
         <v>44403</v>
@@ -1725,16 +1739,16 @@
     </row>
     <row r="39" spans="2:8" ht="15.75" customHeight="1">
       <c r="B39" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F39" s="21">
         <v>44405</v>
@@ -1746,13 +1760,13 @@
     </row>
     <row r="40" spans="2:8" ht="15.75" customHeight="1">
       <c r="B40" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E40" s="16" t="s">
         <v>25</v>
@@ -1767,13 +1781,13 @@
     </row>
     <row r="41" spans="2:8" ht="15.75" customHeight="1">
       <c r="B41" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>25</v>
@@ -1788,7 +1802,7 @@
     </row>
     <row r="42" spans="2:8" ht="15.75" customHeight="1">
       <c r="B42" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="24"/>
@@ -1799,7 +1813,7 @@
     </row>
     <row r="43" spans="2:8" ht="15.75" customHeight="1">
       <c r="B43" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
@@ -1810,13 +1824,13 @@
     </row>
     <row r="44" spans="2:8" ht="15.75" customHeight="1">
       <c r="B44" s="16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E44" s="26" t="s">
         <v>25</v>
@@ -1831,16 +1845,16 @@
     </row>
     <row r="45" spans="2:8" ht="15.75" customHeight="1">
       <c r="B45" s="33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C45" s="34" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>85</v>
+        <v>93</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="F45" s="4">
         <v>44411</v>
@@ -1852,16 +1866,16 @@
     </row>
     <row r="46" spans="2:8" ht="15.75" customHeight="1">
       <c r="B46" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E46" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>100</v>
       </c>
       <c r="F46" s="21">
         <v>44417</v>
@@ -1873,16 +1887,16 @@
     </row>
     <row r="47" spans="2:8" ht="15.75" customHeight="1">
       <c r="B47" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F47" s="21">
         <v>44424</v>
@@ -1894,16 +1908,16 @@
     </row>
     <row r="48" spans="2:8" ht="15.75" customHeight="1">
       <c r="B48" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F48" s="21">
         <v>44424</v>
@@ -1915,16 +1929,16 @@
     </row>
     <row r="49" spans="2:8" ht="15.75" customHeight="1">
       <c r="B49" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F49" s="21">
         <v>44424</v>
@@ -1936,16 +1950,16 @@
     </row>
     <row r="50" spans="2:8" ht="15.75" customHeight="1">
       <c r="B50" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E50" s="43" t="s">
         <v>109</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E50" s="26" t="s">
-        <v>112</v>
       </c>
       <c r="F50" s="21">
         <v>44426</v>
@@ -1957,16 +1971,16 @@
     </row>
     <row r="51" spans="2:8" ht="15.75" customHeight="1">
       <c r="B51" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F51" s="21">
         <v>44428</v>
@@ -1978,16 +1992,16 @@
     </row>
     <row r="52" spans="2:8" ht="15.75" customHeight="1">
       <c r="B52" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F52" s="21">
         <v>44429</v>
@@ -1999,16 +2013,16 @@
     </row>
     <row r="53" spans="2:8" ht="15.75" customHeight="1">
       <c r="B53" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F53" s="21">
         <v>44431</v>
@@ -2020,16 +2034,16 @@
     </row>
     <row r="54" spans="2:8" ht="15.75" customHeight="1">
       <c r="B54" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F54" s="21">
         <v>44434</v>
@@ -2041,16 +2055,16 @@
     </row>
     <row r="55" spans="2:8" ht="15.75" customHeight="1">
       <c r="B55" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F55" s="21">
         <v>44436</v>
@@ -2062,13 +2076,13 @@
     </row>
     <row r="56" spans="2:8" ht="15.75" customHeight="1">
       <c r="B56" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>25</v>
@@ -2083,13 +2097,13 @@
     </row>
     <row r="57" spans="2:8" ht="15.75" customHeight="1">
       <c r="B57" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E57" s="16" t="s">
         <v>25</v>
@@ -2104,7 +2118,7 @@
     </row>
     <row r="58" spans="2:8" ht="15.75" customHeight="1">
       <c r="B58" s="23" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C58" s="12"/>
       <c r="D58" s="24"/>
@@ -3076,6 +3090,6 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se actualizo el cronograma y se eliminaron los archivos de creacion de carpetas
</commit_message>
<xml_diff>
--- a/Documentos/SF/Cronograma/Cronograma de Proyecto.xlsx
+++ b/Documentos/SF/Cronograma/Cronograma de Proyecto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\wong\FiveSolutions\Documentos\SF\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jota\Documents\DESARROLLO JOLLJA\FiveSolutions\Documentos\SF\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF46AE-807B-46CF-9684-A7B31F916288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBD077A-1103-4479-A3E3-9220654DC621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="133">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -421,6 +421,9 @@
   </si>
   <si>
     <t>Tello/DBA, Benavente/BE, Flores/FE</t>
+  </si>
+  <si>
+    <t>ST-PC.xlsx</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -652,6 +655,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -660,10 +668,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,40 +883,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P1004"/>
+  <dimension ref="B1:P1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" customWidth="1"/>
-    <col min="2" max="2" width="52.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.09765625" customWidth="1"/>
-    <col min="6" max="7" width="9.8984375" customWidth="1"/>
-    <col min="8" max="8" width="12.3984375" customWidth="1"/>
-    <col min="9" max="9" width="9.3984375" customWidth="1"/>
-    <col min="10" max="10" width="25.8984375" customWidth="1"/>
-    <col min="11" max="11" width="15.69921875" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="52.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.125" customWidth="1"/>
+    <col min="6" max="7" width="9.875" customWidth="1"/>
+    <col min="8" max="8" width="12.375" customWidth="1"/>
+    <col min="9" max="9" width="9.375" customWidth="1"/>
+    <col min="10" max="10" width="25.875" customWidth="1"/>
+    <col min="11" max="11" width="15.75" customWidth="1"/>
     <col min="12" max="12" width="5.5" customWidth="1"/>
-    <col min="13" max="26" width="9.3984375" customWidth="1"/>
+    <col min="13" max="26" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="14.4">
-      <c r="B1" s="39" t="s">
+    <row r="1" spans="2:16">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-    </row>
-    <row r="2" spans="2:16" ht="14.4">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+    </row>
+    <row r="2" spans="2:16">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -920,7 +924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="14.4">
+    <row r="3" spans="2:16">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -928,7 +932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="14.4">
+    <row r="4" spans="2:16">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -936,7 +940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="14.4">
+    <row r="5" spans="2:16">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -944,7 +948,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="14.4">
+    <row r="6" spans="2:16">
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
@@ -952,7 +956,7 @@
         <v>44349</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="14.4">
+    <row r="7" spans="2:16">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -960,7 +964,7 @@
         <v>44447</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="14.4">
+    <row r="8" spans="2:16">
       <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
@@ -982,17 +986,17 @@
       <c r="H8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="J8" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="42"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="8"/>
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
       <c r="O8" s="9"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="2:16" ht="14.4">
+    <row r="9" spans="2:16">
       <c r="B9" s="12" t="s">
         <v>19</v>
       </c>
@@ -1018,7 +1022,7 @@
       <c r="O9" s="9"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="2:16" ht="14.4">
+    <row r="10" spans="2:16">
       <c r="B10" s="16" t="s">
         <v>22</v>
       </c>
@@ -1052,17 +1056,17 @@
       <c r="O10" s="9"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="2:16" ht="14.4">
-      <c r="B11" s="16" t="s">
+    <row r="11" spans="2:16" s="39" customFormat="1">
+      <c r="B11" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="33" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="4">
@@ -1074,43 +1078,41 @@
       <c r="H11" s="17">
         <v>1</v>
       </c>
-      <c r="J11" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>32</v>
-      </c>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
       <c r="L11" s="8"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="2:16" ht="14.4">
+    <row r="12" spans="2:16">
       <c r="B12" s="16" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="F12" s="4">
-        <v>44350</v>
+        <v>44349</v>
       </c>
       <c r="G12" s="4">
         <v>44356</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="17">
+        <v>1</v>
+      </c>
       <c r="J12" s="19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L12" s="8"/>
       <c r="M12" s="9"/>
@@ -1118,31 +1120,31 @@
       <c r="O12" s="9"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="2:16" ht="14.4">
+    <row r="13" spans="2:16">
       <c r="B13" s="16" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="21">
+        <v>35</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="4">
+        <v>44350</v>
+      </c>
+      <c r="G13" s="4">
         <v>44356</v>
       </c>
-      <c r="G13" s="21">
-        <v>44358</v>
-      </c>
       <c r="H13" s="17"/>
-      <c r="J13" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>44</v>
+      <c r="J13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="9"/>
@@ -1150,18 +1152,18 @@
       <c r="O13" s="9"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="2:16" ht="14.4">
+    <row r="14" spans="2:16">
       <c r="B14" s="16" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F14" s="21">
         <v>44356</v>
@@ -1171,10 +1173,10 @@
       </c>
       <c r="H14" s="17"/>
       <c r="J14" s="16" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="9"/>
@@ -1182,31 +1184,31 @@
       <c r="O14" s="9"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="2:16" ht="14.4">
+    <row r="15" spans="2:16">
       <c r="B15" s="16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>130</v>
+        <v>47</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>48</v>
       </c>
       <c r="F15" s="21">
-        <v>44359</v>
+        <v>44356</v>
       </c>
       <c r="G15" s="21">
-        <v>44362</v>
+        <v>44358</v>
       </c>
       <c r="H15" s="17"/>
       <c r="J15" s="16" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="9"/>
@@ -1214,31 +1216,31 @@
       <c r="O15" s="9"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="2:16" ht="14.4">
-      <c r="B16" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>56</v>
+    <row r="16" spans="2:16">
+      <c r="B16" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="F16" s="21">
-        <v>44363</v>
+        <v>44359</v>
       </c>
       <c r="G16" s="21">
-        <v>44366</v>
+        <v>44362</v>
       </c>
       <c r="H16" s="17"/>
       <c r="J16" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>55</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="9"/>
@@ -1246,43 +1248,47 @@
       <c r="O16" s="9"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="2:16" s="35" customFormat="1" ht="14.4">
+    <row r="17" spans="2:16">
       <c r="B17" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="E17" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>58</v>
       </c>
       <c r="F17" s="21">
         <v>44363</v>
       </c>
       <c r="G17" s="21">
-        <v>44368</v>
+        <v>44366</v>
       </c>
       <c r="H17" s="17"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="37"/>
+      <c r="J17" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="K17" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="L17" s="8"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="2:16" s="35" customFormat="1" ht="14.4">
+    <row r="18" spans="2:16" s="35" customFormat="1">
       <c r="B18" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E18" s="33" t="s">
         <v>58</v>
@@ -1302,15 +1308,15 @@
       <c r="O18" s="9"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="2:16" s="35" customFormat="1" ht="14.4">
+    <row r="19" spans="2:16" s="35" customFormat="1">
       <c r="B19" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E19" s="33" t="s">
         <v>58</v>
@@ -1330,17 +1336,17 @@
       <c r="O19" s="9"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="2:16" ht="14.4">
+    <row r="20" spans="2:16" s="35" customFormat="1">
       <c r="B20" s="19" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>62</v>
+        <v>118</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F20" s="21">
@@ -1350,35 +1356,35 @@
         <v>44368</v>
       </c>
       <c r="H20" s="17"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="9"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="37"/>
       <c r="L20" s="8"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="2:16" ht="14.4">
+    <row r="21" spans="2:16">
       <c r="B21" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>62</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>131</v>
+        <v>63</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>58</v>
       </c>
       <c r="F21" s="21">
-        <v>44367</v>
+        <v>44363</v>
       </c>
       <c r="G21" s="21">
         <v>44368</v>
       </c>
       <c r="H21" s="17"/>
-      <c r="J21" s="20"/>
+      <c r="J21" s="8"/>
       <c r="K21" s="9"/>
       <c r="L21" s="8"/>
       <c r="M21" s="9"/>
@@ -1386,9 +1392,9 @@
       <c r="O21" s="9"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="2:16" ht="14.4">
+    <row r="22" spans="2:16">
       <c r="B22" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>65</v>
@@ -1396,17 +1402,17 @@
       <c r="D22" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>67</v>
+      <c r="E22" s="41" t="s">
+        <v>131</v>
       </c>
       <c r="F22" s="21">
+        <v>44367</v>
+      </c>
+      <c r="G22" s="21">
         <v>44368</v>
       </c>
-      <c r="G22" s="21">
-        <v>44370</v>
-      </c>
       <c r="H22" s="17"/>
-      <c r="J22" s="8"/>
+      <c r="J22" s="20"/>
       <c r="K22" s="9"/>
       <c r="L22" s="8"/>
       <c r="M22" s="9"/>
@@ -1414,9 +1420,9 @@
       <c r="O22" s="9"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="2:16" ht="14.4">
+    <row r="23" spans="2:16">
       <c r="B23" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>65</v>
@@ -1424,14 +1430,14 @@
       <c r="D23" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="22" t="s">
-        <v>69</v>
+      <c r="E23" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="F23" s="21">
+        <v>44368</v>
+      </c>
+      <c r="G23" s="21">
         <v>44370</v>
-      </c>
-      <c r="G23" s="21">
-        <v>44373</v>
       </c>
       <c r="H23" s="17"/>
       <c r="J23" s="8"/>
@@ -1442,9 +1448,9 @@
       <c r="O23" s="9"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="2:16" ht="14.4">
+    <row r="24" spans="2:16">
       <c r="B24" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>65</v>
@@ -1456,58 +1462,65 @@
         <v>69</v>
       </c>
       <c r="F24" s="21">
+        <v>44370</v>
+      </c>
+      <c r="G24" s="21">
         <v>44373</v>
       </c>
-      <c r="G24" s="21">
+      <c r="H24" s="17"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="11"/>
+    </row>
+    <row r="25" spans="2:16">
+      <c r="B25" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="21">
+        <v>44373</v>
+      </c>
+      <c r="G25" s="21">
         <v>44374</v>
       </c>
-      <c r="H24" s="17"/>
-    </row>
-    <row r="25" spans="2:16" ht="14.4">
-      <c r="B25" s="19" t="s">
+      <c r="H25" s="17"/>
+    </row>
+    <row r="26" spans="2:16">
+      <c r="B26" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="16" t="s">
+      <c r="C26" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F26" s="21">
         <v>44375</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G26" s="21">
         <v>44375</v>
       </c>
-      <c r="H25" s="17"/>
-    </row>
-    <row r="26" spans="2:16" ht="14.4">
-      <c r="B26" s="19" t="s">
+      <c r="H26" s="17"/>
+    </row>
+    <row r="27" spans="2:16">
+      <c r="B27" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="21">
-        <v>44376</v>
-      </c>
-      <c r="G26" s="21">
-        <v>44376</v>
-      </c>
-      <c r="H26" s="17"/>
-    </row>
-    <row r="27" spans="2:16" ht="14.4">
-      <c r="B27" s="19" t="s">
-        <v>74</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>65</v>
@@ -1519,89 +1532,89 @@
         <v>25</v>
       </c>
       <c r="F27" s="21">
+        <v>44376</v>
+      </c>
+      <c r="G27" s="21">
+        <v>44376</v>
+      </c>
+      <c r="H27" s="17"/>
+    </row>
+    <row r="28" spans="2:16">
+      <c r="B28" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="21">
         <v>44375</v>
       </c>
-      <c r="G27" s="21">
+      <c r="G28" s="21">
         <v>44375</v>
       </c>
-      <c r="H27" s="16"/>
-    </row>
-    <row r="28" spans="2:16" ht="14.4">
-      <c r="B28" s="23" t="s">
+      <c r="H28" s="16"/>
+    </row>
+    <row r="29" spans="2:16">
+      <c r="B29" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="12"/>
-    </row>
-    <row r="29" spans="2:16" ht="14.4">
-      <c r="B29" s="12" t="s">
+      <c r="C29" s="12"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="12"/>
+    </row>
+    <row r="30" spans="2:16">
+      <c r="B30" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="13"/>
-    </row>
-    <row r="30" spans="2:16" ht="15.75" customHeight="1">
-      <c r="B30" s="16" t="s">
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="2:16" ht="15.75" customHeight="1">
+      <c r="B31" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C31" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D31" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E31" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F31" s="4">
         <v>44379</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G31" s="4">
         <v>44380</v>
       </c>
-      <c r="H30" s="27"/>
-    </row>
-    <row r="31" spans="2:16" ht="15.75" customHeight="1">
-      <c r="B31" s="28" t="s">
+      <c r="H31" s="27"/>
+    </row>
+    <row r="32" spans="2:16" ht="15.75" customHeight="1">
+      <c r="B32" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C32" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D32" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E32" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="F31" s="4">
-        <v>44380</v>
-      </c>
-      <c r="G31" s="4">
-        <v>44383</v>
-      </c>
-      <c r="H31" s="27"/>
-    </row>
-    <row r="32" spans="2:16" s="35" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B32" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="E32" s="33" t="s">
-        <v>58</v>
       </c>
       <c r="F32" s="4">
         <v>44380</v>
@@ -1613,13 +1626,13 @@
     </row>
     <row r="33" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="B33" s="38" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E33" s="33" t="s">
         <v>58</v>
@@ -1634,13 +1647,13 @@
     </row>
     <row r="34" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="B34" s="38" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E34" s="33" t="s">
         <v>58</v>
@@ -1653,30 +1666,30 @@
       </c>
       <c r="H34" s="27"/>
     </row>
-    <row r="35" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B35" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>65</v>
+    <row r="35" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B35" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>126</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E35" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="F35" s="21">
-        <v>44397</v>
-      </c>
-      <c r="G35" s="21">
-        <v>44398</v>
+        <v>129</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="4">
+        <v>44380</v>
+      </c>
+      <c r="G35" s="4">
+        <v>44383</v>
       </c>
       <c r="H35" s="27"/>
     </row>
     <row r="36" spans="2:8" ht="15.75" customHeight="1">
       <c r="B36" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>65</v>
@@ -1684,20 +1697,20 @@
       <c r="D36" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="44" t="s">
-        <v>85</v>
+      <c r="E36" s="31" t="s">
+        <v>84</v>
       </c>
       <c r="F36" s="21">
+        <v>44397</v>
+      </c>
+      <c r="G36" s="21">
         <v>44398</v>
-      </c>
-      <c r="G36" s="21">
-        <v>44400</v>
       </c>
       <c r="H36" s="27"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" customHeight="1">
       <c r="B37" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>65</v>
@@ -1705,20 +1718,20 @@
       <c r="D37" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="22" t="s">
-        <v>69</v>
+      <c r="E37" s="41" t="s">
+        <v>85</v>
       </c>
       <c r="F37" s="21">
+        <v>44398</v>
+      </c>
+      <c r="G37" s="21">
         <v>44400</v>
-      </c>
-      <c r="G37" s="21">
-        <v>44403</v>
       </c>
       <c r="H37" s="27"/>
     </row>
     <row r="38" spans="2:8" ht="15.75" customHeight="1">
       <c r="B38" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>65</v>
@@ -1730,16 +1743,16 @@
         <v>69</v>
       </c>
       <c r="F38" s="21">
+        <v>44400</v>
+      </c>
+      <c r="G38" s="21">
         <v>44403</v>
-      </c>
-      <c r="G38" s="21">
-        <v>44404</v>
       </c>
       <c r="H38" s="27"/>
     </row>
     <row r="39" spans="2:8" ht="15.75" customHeight="1">
       <c r="B39" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>65</v>
@@ -1747,20 +1760,20 @@
       <c r="D39" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="18" t="s">
-        <v>72</v>
+      <c r="E39" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="F39" s="21">
-        <v>44405</v>
+        <v>44403</v>
       </c>
       <c r="G39" s="21">
-        <v>44405</v>
+        <v>44404</v>
       </c>
       <c r="H39" s="27"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" customHeight="1">
       <c r="B40" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>65</v>
@@ -1768,20 +1781,20 @@
       <c r="D40" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E40" s="16" t="s">
-        <v>25</v>
+      <c r="E40" s="18" t="s">
+        <v>72</v>
       </c>
       <c r="F40" s="21">
-        <v>44406</v>
+        <v>44405</v>
       </c>
       <c r="G40" s="21">
-        <v>44406</v>
+        <v>44405</v>
       </c>
       <c r="H40" s="27"/>
     </row>
     <row r="41" spans="2:8" ht="15.75" customHeight="1">
       <c r="B41" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>65</v>
@@ -1793,128 +1806,128 @@
         <v>25</v>
       </c>
       <c r="F41" s="21">
+        <v>44406</v>
+      </c>
+      <c r="G41" s="21">
+        <v>44406</v>
+      </c>
+      <c r="H41" s="27"/>
+    </row>
+    <row r="42" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B42" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="21">
         <v>44405</v>
       </c>
-      <c r="G41" s="21">
+      <c r="G42" s="21">
         <v>44405</v>
       </c>
-      <c r="H41" s="27"/>
-    </row>
-    <row r="42" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B42" s="23" t="s">
+      <c r="H42" s="27"/>
+    </row>
+    <row r="43" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B43" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="12"/>
-    </row>
-    <row r="43" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B43" s="12" t="s">
+      <c r="C43" s="12"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="12"/>
+    </row>
+    <row r="44" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B44" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="13"/>
-    </row>
-    <row r="44" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B44" s="16" t="s">
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="13"/>
+    </row>
+    <row r="45" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B45" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C45" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D45" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E44" s="26" t="s">
+      <c r="E45" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F45" s="4">
         <v>44410</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G45" s="4">
         <v>44411</v>
       </c>
-      <c r="H44" s="27"/>
-    </row>
-    <row r="45" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B45" s="33" t="s">
+      <c r="H45" s="27"/>
+    </row>
+    <row r="46" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B46" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C46" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D46" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="E45" s="19" t="s">
+      <c r="E46" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F46" s="4">
         <v>44411</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G46" s="4">
         <v>44414</v>
-      </c>
-      <c r="H45" s="27"/>
-    </row>
-    <row r="46" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B46" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F46" s="21">
-        <v>44417</v>
-      </c>
-      <c r="G46" s="21">
-        <v>44419</v>
       </c>
       <c r="H46" s="27"/>
     </row>
     <row r="47" spans="2:8" ht="15.75" customHeight="1">
       <c r="B47" s="16" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>58</v>
+        <v>96</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="F47" s="21">
-        <v>44424</v>
+        <v>44417</v>
       </c>
       <c r="G47" s="21">
-        <v>44426</v>
+        <v>44419</v>
       </c>
       <c r="H47" s="27"/>
     </row>
     <row r="48" spans="2:8" ht="15.75" customHeight="1">
       <c r="B48" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>96</v>
+        <v>99</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>100</v>
       </c>
       <c r="E48" s="16" t="s">
         <v>58</v>
@@ -1929,13 +1942,13 @@
     </row>
     <row r="49" spans="2:8" ht="15.75" customHeight="1">
       <c r="B49" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="E49" s="16" t="s">
         <v>58</v>
@@ -1950,49 +1963,49 @@
     </row>
     <row r="50" spans="2:8" ht="15.75" customHeight="1">
       <c r="B50" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F50" s="21">
+        <v>44424</v>
+      </c>
+      <c r="G50" s="21">
+        <v>44426</v>
+      </c>
+      <c r="H50" s="27"/>
+    </row>
+    <row r="51" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B51" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C51" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D50" s="22" t="s">
+      <c r="D51" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="E50" s="43" t="s">
+      <c r="E51" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="F50" s="21">
+      <c r="F51" s="21">
         <v>44426</v>
       </c>
-      <c r="G50" s="21">
+      <c r="G51" s="21">
         <v>44428</v>
-      </c>
-      <c r="H50" s="27"/>
-    </row>
-    <row r="51" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B51" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E51" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="F51" s="21">
-        <v>44428</v>
-      </c>
-      <c r="G51" s="21">
-        <v>44429</v>
       </c>
       <c r="H51" s="27"/>
     </row>
     <row r="52" spans="2:8" ht="15.75" customHeight="1">
       <c r="B52" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>65</v>
@@ -2001,19 +2014,19 @@
         <v>65</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="F52" s="21">
+        <v>44428</v>
+      </c>
+      <c r="G52" s="21">
         <v>44429</v>
-      </c>
-      <c r="G52" s="21">
-        <v>44431</v>
       </c>
       <c r="H52" s="27"/>
     </row>
     <row r="53" spans="2:8" ht="15.75" customHeight="1">
       <c r="B53" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>65</v>
@@ -2022,19 +2035,19 @@
         <v>65</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="F53" s="21">
+        <v>44429</v>
+      </c>
+      <c r="G53" s="21">
         <v>44431</v>
-      </c>
-      <c r="G53" s="21">
-        <v>44434</v>
       </c>
       <c r="H53" s="27"/>
     </row>
     <row r="54" spans="2:8" ht="15.75" customHeight="1">
       <c r="B54" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>65</v>
@@ -2042,20 +2055,20 @@
       <c r="D54" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E54" s="22" t="s">
+      <c r="E54" s="16" t="s">
         <v>69</v>
       </c>
       <c r="F54" s="21">
+        <v>44431</v>
+      </c>
+      <c r="G54" s="21">
         <v>44434</v>
-      </c>
-      <c r="G54" s="21">
-        <v>44435</v>
       </c>
       <c r="H54" s="27"/>
     </row>
     <row r="55" spans="2:8" ht="15.75" customHeight="1">
       <c r="B55" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C55" s="16" t="s">
         <v>65</v>
@@ -2063,20 +2076,20 @@
       <c r="D55" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E55" s="18" t="s">
-        <v>72</v>
+      <c r="E55" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="F55" s="21">
-        <v>44436</v>
+        <v>44434</v>
       </c>
       <c r="G55" s="21">
-        <v>44436</v>
+        <v>44435</v>
       </c>
       <c r="H55" s="27"/>
     </row>
     <row r="56" spans="2:8" ht="15.75" customHeight="1">
       <c r="B56" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C56" s="16" t="s">
         <v>65</v>
@@ -2084,20 +2097,20 @@
       <c r="D56" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E56" s="16" t="s">
-        <v>25</v>
+      <c r="E56" s="18" t="s">
+        <v>72</v>
       </c>
       <c r="F56" s="21">
-        <v>44437</v>
+        <v>44436</v>
       </c>
       <c r="G56" s="21">
-        <v>44437</v>
+        <v>44436</v>
       </c>
       <c r="H56" s="27"/>
     </row>
     <row r="57" spans="2:8" ht="15.75" customHeight="1">
       <c r="B57" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>65</v>
@@ -2109,34 +2122,54 @@
         <v>25</v>
       </c>
       <c r="F57" s="21">
+        <v>44437</v>
+      </c>
+      <c r="G57" s="21">
+        <v>44437</v>
+      </c>
+      <c r="H57" s="27"/>
+    </row>
+    <row r="58" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B58" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" s="21">
         <v>44436</v>
       </c>
-      <c r="G57" s="21">
+      <c r="G58" s="21">
         <v>44436</v>
       </c>
-      <c r="H57" s="27"/>
-    </row>
-    <row r="58" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B58" s="23" t="s">
+      <c r="H58" s="27"/>
+    </row>
+    <row r="59" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B59" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C58" s="12"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="12"/>
-    </row>
-    <row r="59" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B59" s="12"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="24"/>
       <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="15"/>
-    </row>
-    <row r="60" spans="2:8" ht="15.75" customHeight="1"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="12"/>
+    </row>
+    <row r="60" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B60" s="12"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="15"/>
+    </row>
     <row r="61" spans="2:8" ht="15.75" customHeight="1"/>
     <row r="62" spans="2:8" ht="15.75" customHeight="1"/>
     <row r="63" spans="2:8" ht="15.75" customHeight="1"/>
@@ -3081,6 +3114,7 @@
     <row r="1002" ht="15.75" customHeight="1"/>
     <row r="1003" ht="15.75" customHeight="1"/>
     <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:H1"/>

</xml_diff>